<commit_message>
balance sheet data bucketing almost done 20 maa
</commit_message>
<xml_diff>
--- a/output/599060e9-8b46-46ec-87b9-c79cde8a82b7/599060e9-8b46-46ec-87b9-c79cde8a82b7_main_pages.xlsx
+++ b/output/599060e9-8b46-46ec-87b9-c79cde8a82b7/599060e9-8b46-46ec-87b9-c79cde8a82b7_main_pages.xlsx
@@ -703,6 +703,12 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2" t="s">
         <v>54</v>
       </c>
@@ -714,6 +720,12 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="E3" t="s">
         <v>54</v>
       </c>
@@ -788,6 +800,9 @@
       <c r="B7" t="s">
         <v>42</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="D7">
         <v>29753</v>
       </c>
@@ -859,6 +874,12 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="E11" t="s">
         <v>54</v>
       </c>
@@ -933,6 +954,9 @@
       <c r="B15" t="s">
         <v>42</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
       <c r="D15">
         <v>12453</v>
       </c>
@@ -970,6 +994,9 @@
       <c r="B17" t="s">
         <v>44</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
       <c r="D17">
         <v>678</v>
       </c>
@@ -1018,6 +1045,12 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
       <c r="E20" t="s">
         <v>54</v>
       </c>
@@ -1029,6 +1062,12 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
       <c r="E21" t="s">
         <v>55</v>
       </c>
@@ -1060,6 +1099,9 @@
       <c r="B23" t="s">
         <v>49</v>
       </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
       <c r="D23">
         <v>4000</v>
       </c>
@@ -1100,6 +1142,9 @@
       <c r="C25">
         <v>2935</v>
       </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
       <c r="E25" t="s">
         <v>55</v>
       </c>
@@ -1148,6 +1193,12 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
       <c r="E28" t="s">
         <v>55</v>
       </c>
@@ -1286,6 +1337,12 @@
     <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>34</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
       </c>
       <c r="E36" t="s">
         <v>55</v>
@@ -1533,6 +1590,9 @@
       <c r="C12">
         <v>-25567</v>
       </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
@@ -1607,6 +1667,12 @@
       <c r="A2" t="s">
         <v>78</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2" t="s">
         <v>97</v>
       </c>
@@ -1713,6 +1779,12 @@
       <c r="A10" t="s">
         <v>86</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="E10" t="s">
         <v>98</v>
       </c>
@@ -1749,6 +1821,12 @@
       <c r="A13" t="s">
         <v>89</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13" t="s">
         <v>99</v>
       </c>
@@ -1770,6 +1848,9 @@
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>91</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
       <c r="D15">
         <v>33500</v>

</xml_diff>